<commit_message>
Computed column Cat_tot for each sheet
I also deleted these empty sheets
G1S1
S1 S3
S2S2
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/PLITs/extraction/PLIT_AWA.xlsx
+++ b/Multi-taxa_data/PLITs/extraction/PLIT_AWA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\COMUNE\STUDIO.LAVORO\IMBRSea\Thesis\StatAnalysis\Multi-taxa_data\PLITs\extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243B9332-73C0-4DAA-96F6-B66777F8BF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6736B8-17D0-4D35-9097-0DCD9D162BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D1" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="359">
   <si>
     <t>D1</t>
   </si>
@@ -1514,7 +1514,9 @@
   </sheetPr>
   <dimension ref="A1:P166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2818,17 +2820,11 @@
         <v>2720</v>
       </c>
       <c r="B63" s="10"/>
-      <c r="C63" s="19">
-        <f>SUM(C5:C62)</f>
-        <v>2650</v>
-      </c>
+      <c r="C63" s="19"/>
       <c r="D63" s="10"/>
       <c r="K63" s="10"/>
     </row>
     <row r="64" spans="1:12">
-      <c r="A64" s="10" t="s">
-        <v>90</v>
-      </c>
       <c r="B64" s="10"/>
       <c r="D64" s="10"/>
       <c r="E64" s="10"/>
@@ -3453,7 +3449,9 @@
   </sheetPr>
   <dimension ref="A1:X172"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -5218,17 +5216,12 @@
         <v>2750</v>
       </c>
       <c r="B83" s="10"/>
-      <c r="C83" s="11">
-        <f>SUM(C5:C82)</f>
-        <v>2716</v>
-      </c>
+      <c r="C83" s="11"/>
       <c r="D83" s="10"/>
       <c r="K83" s="10"/>
     </row>
     <row r="84" spans="1:12">
-      <c r="A84" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="A84" s="10"/>
       <c r="B84" s="10"/>
       <c r="D84" s="10"/>
       <c r="K84" s="10"/>
@@ -5780,7 +5773,9 @@
   </sheetPr>
   <dimension ref="A1:X71"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -7276,15 +7271,10 @@
       <c r="A70" s="11">
         <v>2740</v>
       </c>
-      <c r="C70" s="11">
-        <f>SUM(C5:C69)</f>
-        <v>2677</v>
-      </c>
+      <c r="C70" s="11"/>
     </row>
     <row r="71" spans="1:11">
-      <c r="A71" s="11" t="s">
-        <v>90</v>
-      </c>
+      <c r="A71" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7298,7 +7288,9 @@
   </sheetPr>
   <dimension ref="A1:X252"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -8546,16 +8538,13 @@
       <c r="A55" s="11">
         <v>2790</v>
       </c>
+      <c r="B55" s="11"/>
       <c r="C55" s="11">
         <f>SUM(C5:C54)</f>
         <v>2720</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
+    <row r="56" spans="1:11"/>
     <row r="243" spans="13:17">
       <c r="M243" s="10"/>
       <c r="N243" s="10"/>
@@ -8638,7 +8627,7 @@
   </sheetPr>
   <dimension ref="A1:X77"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A69" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -10281,7 +10270,9 @@
   </sheetPr>
   <dimension ref="A1:X256"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -11821,9 +11812,7 @@
       <c r="K69" s="10"/>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="A70" s="10"/>
       <c r="B70" s="10"/>
       <c r="D70" s="10"/>
       <c r="K70" s="10"/>

</xml_diff>

<commit_message>
Computed Cat_tot and corrected negative cover values
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/PLITs/extraction/PLIT_AWA.xlsx
+++ b/Multi-taxa_data/PLITs/extraction/PLIT_AWA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\COMUNE\STUDIO.LAVORO\IMBRSea\Thesis\StatAnalysis\Multi-taxa_data\PLITs\extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6736B8-17D0-4D35-9097-0DCD9D162BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73853332-5002-4043-BE2C-9AE7822A8BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D1" sheetId="2" r:id="rId1"/>
@@ -7288,8 +7288,8 @@
   </sheetPr>
   <dimension ref="A1:X252"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
@@ -8539,10 +8539,7 @@
         <v>2790</v>
       </c>
       <c r="B55" s="11"/>
-      <c r="C55" s="11">
-        <f>SUM(C5:C54)</f>
-        <v>2720</v>
-      </c>
+      <c r="C55" s="11"/>
     </row>
     <row r="56" spans="1:11"/>
     <row r="243" spans="13:17">
@@ -8627,1651 +8624,8 @@
   </sheetPr>
   <dimension ref="A1:X77"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="8.59765625" customWidth="1"/>
-    <col min="2" max="2" width="19.59765625" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" customWidth="1"/>
-    <col min="4" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="8.59765625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="11.69921875" customWidth="1"/>
-    <col min="9" max="10" width="8.59765625" customWidth="1"/>
-    <col min="11" max="11" width="13.3984375" customWidth="1"/>
-    <col min="12" max="14" width="8.59765625" customWidth="1"/>
-    <col min="16" max="16" width="8.796875" customWidth="1"/>
-    <col min="17" max="25" width="8.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24">
-      <c r="A1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="3">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="R3" s="10"/>
-    </row>
-    <row r="4" spans="1:24">
-      <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-    </row>
-    <row r="5" spans="1:24">
-      <c r="A5" s="11">
-        <v>30</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="11">
-        <f t="shared" ref="C5:C75" si="0">A6-A5</f>
-        <v>124</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="O5" s="10">
-        <f>SUMIF($B$5:$B$75,"hard_coral",$C$5:$C$75)</f>
-        <v>189</v>
-      </c>
-      <c r="P5" s="14">
-        <f t="shared" ref="P5:P15" si="1">(O5/$O$16)*100</f>
-        <v>7.3114119922630563</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="S5" s="11">
-        <v>2252</v>
-      </c>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-    </row>
-    <row r="6" spans="1:24">
-      <c r="A6" s="11">
-        <v>154</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O6" s="10">
-        <f>SUMIF($B$5:$B$75,"algae",$C$5:$C$75)</f>
-        <v>2252</v>
-      </c>
-      <c r="P6" s="14">
-        <f t="shared" si="1"/>
-        <v>87.117988394584131</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="S6" s="10">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
-      <c r="A7" s="11">
-        <v>157</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="11">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="O7" s="10">
-        <f>SUMIF($B$5:$B$75,"soft_coral",$C$5:$C$75)</f>
-        <v>3</v>
-      </c>
-      <c r="P7" s="14">
-        <f t="shared" si="1"/>
-        <v>0.11605415860735009</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="S7" s="10">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
-      <c r="A8" s="11">
-        <v>209</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="11">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="O8" s="10">
-        <f>SUMIF($B$5:$B$75,"boulder",$C$5:$C$75)</f>
-        <v>58</v>
-      </c>
-      <c r="P8" s="14">
-        <f t="shared" si="1"/>
-        <v>2.2437137330754351</v>
-      </c>
-      <c r="R8" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="S8" s="11">
-        <v>0</v>
-      </c>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-    </row>
-    <row r="9" spans="1:24">
-      <c r="A9" s="11">
-        <v>216</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="11">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O9" s="10">
-        <f>SUMIF($B$5:$B$75,"rubble",$C$5:$C$75)</f>
-        <v>3</v>
-      </c>
-      <c r="P9" s="14">
-        <f t="shared" si="1"/>
-        <v>0.11605415860735009</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S9" s="10">
-        <v>3</v>
-      </c>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-    </row>
-    <row r="10" spans="1:24">
-      <c r="A10" s="11">
-        <v>225</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="11">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="O10" s="10">
-        <f>SUMIF($B$5:$B$75,"sand",$C$5:$C$75)</f>
-        <v>61</v>
-      </c>
-      <c r="P10" s="14">
-        <f t="shared" si="1"/>
-        <v>2.3597678916827856</v>
-      </c>
-      <c r="R10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="S10" s="11">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24">
-      <c r="A11" s="11">
-        <v>233</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="11">
-        <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="N11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="O11" s="10">
-        <f>SUMIF($B$5:$B$75,"sponge",$C$5:$C$75)</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S11" s="11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24">
-      <c r="A12" s="11">
-        <v>321</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="N12" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="O12" s="10">
-        <f>SUMIF($B$5:$B$75,"other",$C$5:$C$75)</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="S12" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24">
-      <c r="A13" s="11">
-        <v>322</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="11">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="N13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="O13" s="10">
-        <f>SUMIF($B$5:$B$75,"unknown",$C$5:$C$75)</f>
-        <v>10</v>
-      </c>
-      <c r="P13" s="14">
-        <f t="shared" si="1"/>
-        <v>0.38684719535783368</v>
-      </c>
-      <c r="R13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="S13" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24">
-      <c r="A14" s="11">
-        <v>366</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="N14" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="O14" s="10">
-        <f>SUMIF($B$5:$B$75,"shadow",$C$5:$C$75)</f>
-        <v>9</v>
-      </c>
-      <c r="P14" s="14">
-        <f t="shared" si="1"/>
-        <v>0.34816247582205029</v>
-      </c>
-      <c r="R14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="S14" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24">
-      <c r="A15" s="11">
-        <v>367</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="11">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="N15" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="O15" s="10">
-        <f>SUMIF($B$5:$B$75,"zoanthids",$C$5:$C$75)</f>
-        <v>0</v>
-      </c>
-      <c r="P15" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="S15" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24">
-      <c r="A16" s="11">
-        <v>375</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="O16" s="16">
-        <f t="shared" ref="O16:P16" si="2">SUM(O5:O15)</f>
-        <v>2585</v>
-      </c>
-      <c r="P16" s="17">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="11">
-        <v>380</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="11">
-        <f t="shared" si="0"/>
-        <v>127</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="11">
-        <v>507</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="11">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="N18" s="11" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="11">
-        <v>519</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="11">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="N19" s="16">
-        <f>C76-SUMIF(B5:B75,"missing",C5:C75)</f>
-        <v>2585</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="11">
-        <v>535</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="11">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="11">
-        <v>565</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K21" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="N21" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="11">
-        <v>568</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="11">
-        <v>571</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="11">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="11">
-        <v>598</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="11">
-        <v>603</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="11" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="11">
-        <v>608</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="11">
-        <f t="shared" si="0"/>
-        <v>116</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="11">
-        <v>724</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K27" s="11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="11">
-        <v>729</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="11">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="11">
-        <v>735</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K29" s="11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="11">
-        <v>737</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="11">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" s="11">
-        <v>774</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="25" t="s">
-        <v>272</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="11">
-        <v>778</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="11">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="11">
-        <v>839</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K33" s="11" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="11">
-        <v>842</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="11">
-        <f t="shared" si="0"/>
-        <v>181</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="11">
-        <v>1023</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D35" s="23"/>
-      <c r="K35" s="11" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="11">
-        <v>1028</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="11">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K36" s="11" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="11">
-        <v>1065</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>279</v>
-      </c>
-      <c r="C37" s="11">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="L37" s="26" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="11">
-        <v>1080</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="11">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K38" s="11" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="11">
-        <v>1109</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K39" s="11" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="11">
-        <v>1113</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="11">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K40" s="11" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="A41" s="11">
-        <v>1154</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="11">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K41" s="11" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="A42" s="11">
-        <v>1188</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="11">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K42" s="11" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="11">
-        <v>1273</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K43" s="11" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="A44" s="11">
-        <v>1276</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="11">
-        <f t="shared" si="0"/>
-        <v>154</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K44" s="11" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="A45" s="11">
-        <v>1430</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K45" s="11" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="A46" s="11">
-        <v>1433</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="11">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K46" s="11" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="11">
-        <v>1482</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="11">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K47" s="11" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="11">
-        <v>1495</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="11">
-        <f t="shared" si="0"/>
-        <v>113</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K48" s="11" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="11">
-        <v>1608</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="11">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K49" s="11" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="11">
-        <v>1619</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="11">
-        <v>1622</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K51" s="11" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="11">
-        <v>1625</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="11">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K52" s="11" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="11">
-        <v>1641</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="11">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K53" s="11" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="11">
-        <v>1740</v>
-      </c>
-      <c r="B54" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K54" s="11" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="11">
-        <v>1743</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55" s="11">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K55" s="11" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="11">
-        <v>1818</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C56" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K56" s="11" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11">
-      <c r="A57" s="11">
-        <v>1820</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C57" s="11">
-        <f t="shared" si="0"/>
-        <v>83</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K57" s="11" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="A58" s="11">
-        <v>1903</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" s="11">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="D58" s="23"/>
-      <c r="K58" s="11" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="A59" s="11">
-        <v>1920</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="11">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K59" s="11" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
-      <c r="A60" s="11">
-        <v>1960</v>
-      </c>
-      <c r="B60" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C60" s="11">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K60" s="11" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="A61" s="11">
-        <v>1967</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C61" s="11">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K61" s="11" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="11">
-        <v>1982</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C62" s="11">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K62" s="11" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11">
-      <c r="A63" s="11">
-        <v>2015</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C63" s="11">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="K63" s="11" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11">
-      <c r="A64" s="11">
-        <v>2062</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C64" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K64" s="11" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12">
-      <c r="A65" s="11">
-        <v>2067</v>
-      </c>
-      <c r="B65" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C65" s="11">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K65" s="11" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12">
-      <c r="A66" s="11">
-        <v>2074</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="11">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K66" s="11" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12">
-      <c r="A67" s="11">
-        <v>2080</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" s="11">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K67" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="L67" s="23" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12">
-      <c r="A68" s="11">
-        <v>2103</v>
-      </c>
-      <c r="B68" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C68" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D68" s="23"/>
-      <c r="K68" s="11" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12">
-      <c r="A69" s="11">
-        <v>2108</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C69" s="11">
-        <f t="shared" si="0"/>
-        <v>104</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K69" s="11" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12">
-      <c r="A70" s="11">
-        <v>2212</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C70" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K70" s="11" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12">
-      <c r="A71" s="11">
-        <v>2217</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C71" s="11">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="D71" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K71" s="11" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12">
-      <c r="A72" s="11">
-        <v>2255</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C72" s="11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K72" s="11" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12">
-      <c r="A73" s="11">
-        <v>2265</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C73" s="11">
-        <f t="shared" si="0"/>
-        <v>235</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K73" s="11" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12">
-      <c r="A74" s="11">
-        <v>2500</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C74" s="11">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K74" s="11" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12">
-      <c r="A75" s="11">
-        <v>2512</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C75" s="11">
-        <f t="shared" si="0"/>
-        <v>118</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K75" s="11" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12">
-      <c r="A76" s="11">
-        <v>2630</v>
-      </c>
-      <c r="C76" s="11">
-        <f>SUM(C5:C75)</f>
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12">
-      <c r="A77" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:X256"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
@@ -10295,7 +8649,7 @@
         <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -10313,7 +8667,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -10400,40 +8754,38 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="10">
-        <v>0</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="11">
+        <v>30</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="11">
-        <f t="shared" ref="C5:C68" si="0">A6-A5</f>
-        <v>155</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="10" t="s">
-        <v>312</v>
+        <f t="shared" ref="C5:C75" si="0">A6-A5</f>
+        <v>124</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>251</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="O5" s="10">
-        <f>SUMIF($B$5:$B$68,"hard_coral",$C$5:$C$68)</f>
-        <v>184</v>
+        <f>SUMIF($B$5:$B$75,"hard_coral",$C$5:$C$75)</f>
+        <v>189</v>
       </c>
       <c r="P5" s="14">
         <f t="shared" ref="P5:P15" si="1">(O5/$O$16)*100</f>
-        <v>7.3717948717948723</v>
+        <v>7.3114119922630563</v>
       </c>
       <c r="R5" s="11" t="s">
         <v>11</v>
       </c>
       <c r="S5" s="11">
-        <v>2209</v>
+        <v>2252</v>
       </c>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
@@ -10442,6 +8794,1650 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24">
+      <c r="A6" s="11">
+        <v>154</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O6" s="10">
+        <f>SUMIF($B$5:$B$75,"algae",$C$5:$C$75)</f>
+        <v>2252</v>
+      </c>
+      <c r="P6" s="14">
+        <f t="shared" si="1"/>
+        <v>87.117988394584131</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" s="10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" s="11">
+        <v>157</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="11">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="10">
+        <f>SUMIF($B$5:$B$75,"soft_coral",$C$5:$C$75)</f>
+        <v>3</v>
+      </c>
+      <c r="P7" s="14">
+        <f t="shared" si="1"/>
+        <v>0.11605415860735009</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="S7" s="10">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="A8" s="11">
+        <v>209</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="10">
+        <f>SUMIF($B$5:$B$75,"boulder",$C$5:$C$75)</f>
+        <v>58</v>
+      </c>
+      <c r="P8" s="14">
+        <f t="shared" si="1"/>
+        <v>2.2437137330754351</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="S8" s="11">
+        <v>0</v>
+      </c>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" s="11">
+        <v>216</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O9" s="10">
+        <f>SUMIF($B$5:$B$75,"rubble",$C$5:$C$75)</f>
+        <v>3</v>
+      </c>
+      <c r="P9" s="14">
+        <f t="shared" si="1"/>
+        <v>0.11605415860735009</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="S9" s="10">
+        <v>3</v>
+      </c>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10" s="11">
+        <v>225</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" s="10">
+        <f>SUMIF($B$5:$B$75,"sand",$C$5:$C$75)</f>
+        <v>61</v>
+      </c>
+      <c r="P10" s="14">
+        <f t="shared" si="1"/>
+        <v>2.3597678916827856</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="S10" s="11">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" s="11">
+        <v>233</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="11">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" s="10">
+        <f>SUMIF($B$5:$B$75,"sponge",$C$5:$C$75)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S11" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" s="11">
+        <v>321</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="10">
+        <f>SUMIF($B$5:$B$75,"other",$C$5:$C$75)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S12" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13" s="11">
+        <v>322</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="11">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" s="10">
+        <f>SUMIF($B$5:$B$75,"unknown",$C$5:$C$75)</f>
+        <v>10</v>
+      </c>
+      <c r="P13" s="14">
+        <f t="shared" si="1"/>
+        <v>0.38684719535783368</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="S13" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="A14" s="11">
+        <v>366</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O14" s="10">
+        <f>SUMIF($B$5:$B$75,"shadow",$C$5:$C$75)</f>
+        <v>9</v>
+      </c>
+      <c r="P14" s="14">
+        <f t="shared" si="1"/>
+        <v>0.34816247582205029</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="S14" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="A15" s="11">
+        <v>367</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="O15" s="10">
+        <f>SUMIF($B$5:$B$75,"zoanthids",$C$5:$C$75)</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="S15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16" s="11">
+        <v>375</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="O16" s="16">
+        <f t="shared" ref="O16:P16" si="2">SUM(O5:O15)</f>
+        <v>2585</v>
+      </c>
+      <c r="P16" s="17">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="11">
+        <v>380</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="11">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="11">
+        <v>507</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="11">
+        <v>519</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="11">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="N19" s="16">
+        <f>C76-SUMIF(B5:B75,"missing",C5:C75)</f>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="11">
+        <v>535</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="11">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="11">
+        <v>565</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="11">
+        <v>568</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="11">
+        <v>571</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="11">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="11">
+        <v>598</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="11">
+        <v>603</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="11">
+        <v>608</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="11">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="11">
+        <v>724</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="11">
+        <v>729</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="11">
+        <v>735</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="11">
+        <v>737</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="11">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="11">
+        <v>774</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="11">
+        <v>778</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="11">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="11">
+        <v>839</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="11">
+        <v>842</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="11">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="11">
+        <v>1023</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D35" s="23"/>
+      <c r="K35" s="11" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="11">
+        <v>1028</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="11">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="11">
+        <v>1065</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="C37" s="11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K37" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L37" s="26" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="11">
+        <v>1080</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="11">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="11">
+        <v>1109</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K39" s="11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="11">
+        <v>1113</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="11">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="11">
+        <v>1154</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="11">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K41" s="11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="11">
+        <v>1188</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="11">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K42" s="11" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="11">
+        <v>1273</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="11">
+        <v>1276</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="11">
+        <f t="shared" si="0"/>
+        <v>154</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K44" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="11">
+        <v>1430</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K45" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="11">
+        <v>1433</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="11">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K46" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="11">
+        <v>1482</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="11">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K47" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="11">
+        <v>1495</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="11">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K48" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="11">
+        <v>1608</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="11">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K49" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="11">
+        <v>1619</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="11">
+        <v>1622</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K51" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="11">
+        <v>1625</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="11">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="11">
+        <v>1641</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="11">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K53" s="11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="11">
+        <v>1740</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K54" s="11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="11">
+        <v>1743</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="11">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K55" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="11">
+        <v>1818</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C56" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K56" s="11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="11">
+        <v>1820</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="11">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K57" s="11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="11">
+        <v>1903</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D58" s="23"/>
+      <c r="K58" s="11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="11">
+        <v>1920</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="11">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K59" s="11" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="11">
+        <v>1960</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C60" s="11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K60" s="11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="11">
+        <v>1967</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K61" s="11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="11">
+        <v>1982</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="11">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K62" s="11" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="11">
+        <v>2015</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="11">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K63" s="11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="11">
+        <v>2062</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K64" s="11" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="11">
+        <v>2067</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K65" s="11" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="11">
+        <v>2074</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K66" s="11" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="11">
+        <v>2080</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="11">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K67" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="L67" s="23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="11">
+        <v>2103</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D68" s="23"/>
+      <c r="K68" s="11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="11">
+        <v>2108</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="11">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K69" s="11" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="11">
+        <v>2212</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K70" s="11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="11">
+        <v>2217</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="11">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K71" s="11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="11">
+        <v>2255</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K72" s="11" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" s="11">
+        <v>2265</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="11">
+        <f t="shared" si="0"/>
+        <v>235</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K73" s="11" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="11">
+        <v>2500</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" s="11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K74" s="11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="11">
+        <v>2512</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" s="11">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K75" s="11" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" s="11">
+        <v>2630</v>
+      </c>
+      <c r="C76" s="11"/>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:X256"/>
+  <sheetViews>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="8.59765625" customWidth="1"/>
+    <col min="2" max="2" width="19.59765625" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" customWidth="1"/>
+    <col min="4" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="8.59765625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="11.69921875" customWidth="1"/>
+    <col min="9" max="10" width="8.59765625" customWidth="1"/>
+    <col min="11" max="11" width="13.3984375" customWidth="1"/>
+    <col min="12" max="14" width="8.59765625" customWidth="1"/>
+    <col min="16" max="16" width="8.796875" customWidth="1"/>
+    <col min="17" max="25" width="8.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="R3" s="10"/>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" s="10">
+        <v>0</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="11">
+        <f t="shared" ref="C5:C68" si="0">A6-A5</f>
+        <v>155</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="10">
+        <f>SUMIF($B$5:$B$68,"hard_coral",$C$5:$C$68)</f>
+        <v>184</v>
+      </c>
+      <c r="P5" s="14">
+        <f t="shared" ref="P5:P15" si="1">(O5/$O$16)*100</f>
+        <v>7.3717948717948723</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="S5" s="11">
+        <v>2209</v>
+      </c>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" s="10">
         <v>155</v>
       </c>
@@ -10898,7 +10894,7 @@
       <c r="L19" s="10"/>
       <c r="N19" s="16">
         <f>C69-SUMIF(B5:B68,"missing",C5:C68)</f>
-        <v>2496</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -11804,10 +11800,7 @@
         <v>2516</v>
       </c>
       <c r="B69" s="10"/>
-      <c r="C69" s="11">
-        <f>SUM(C5:C68)</f>
-        <v>2516</v>
-      </c>
+      <c r="C69" s="11"/>
       <c r="D69" s="10"/>
       <c r="K69" s="10"/>
     </row>

</xml_diff>